<commit_message>
added a percent increase rent field
</commit_message>
<xml_diff>
--- a/docs/target_training_fields.xlsx
+++ b/docs/target_training_fields.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="156">
   <si>
     <t>Decision</t>
   </si>
@@ -478,6 +478,21 @@
   </si>
   <si>
     <t>Training table:</t>
+  </si>
+  <si>
+    <t>percent_increase_neighborhood_median_rent</t>
+  </si>
+  <si>
+    <t>percent_increase_neighborhood_upper_rent</t>
+  </si>
+  <si>
+    <t>percent_increase_neighborhood_lower_rent</t>
+  </si>
+  <si>
+    <t>calculate increase from 2009 to 2014 rent in the acs_rent_median table, e.g. (rent '14 - rent '09) / rent '09</t>
+  </si>
+  <si>
+    <t>calculate as above</t>
   </si>
 </sst>
 </file>
@@ -516,7 +531,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +574,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -581,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -594,6 +615,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,173 +1347,197 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>31</v>
+      <c r="A50" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>32</v>
+      <c r="A51" s="12" t="s">
+        <v>152</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>33</v>
+      <c r="A52" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>34</v>
       </c>
-      <c r="D53" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B57" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>83</v>
+      <c r="A60" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B77" t="s">
-        <v>137</v>
+      <c r="A77" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>